<commit_message>
Added item analysis and interpretation it. Save the results to the same excel file. Also formatted the original excel test results
</commit_message>
<xml_diff>
--- a/Data analytics/Language tests/Data/one_test_descriptive_stats.xlsx
+++ b/Data analytics/Language tests/Data/one_test_descriptive_stats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="84">
   <si>
     <t>Student</t>
   </si>
@@ -179,6 +179,30 @@
   </si>
   <si>
     <t>Student30</t>
+  </si>
+  <si>
+    <t>Item facility</t>
+  </si>
+  <si>
+    <t>IF</t>
+  </si>
+  <si>
+    <t>IF(upper)</t>
+  </si>
+  <si>
+    <t>IF(lower)</t>
+  </si>
+  <si>
+    <t>Item discrimination</t>
+  </si>
+  <si>
+    <t>ID(UL)</t>
+  </si>
+  <si>
+    <t>r(p-bis)</t>
+  </si>
+  <si>
+    <t>Flagged</t>
   </si>
   <si>
     <t>Statistics</t>
@@ -320,13 +344,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>125689</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>24825</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -344,7 +368,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4267200" y="6286500"/>
+          <a:off x="4267200" y="9144000"/>
           <a:ext cx="10488889" cy="4596825"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -355,6 +379,40 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Y31" totalsRowShown="0">
+  <autoFilter ref="A1:Y31"/>
+  <tableColumns count="25">
+    <tableColumn id="1" name="Student"/>
+    <tableColumn id="2" name="Q01"/>
+    <tableColumn id="3" name="Q02"/>
+    <tableColumn id="4" name="Q03"/>
+    <tableColumn id="5" name="Q04"/>
+    <tableColumn id="6" name="Q05"/>
+    <tableColumn id="7" name="Q06"/>
+    <tableColumn id="8" name="Q07"/>
+    <tableColumn id="9" name="Q08"/>
+    <tableColumn id="10" name="Q09"/>
+    <tableColumn id="11" name="Q10"/>
+    <tableColumn id="12" name="Q11"/>
+    <tableColumn id="13" name="Q12"/>
+    <tableColumn id="14" name="Q13"/>
+    <tableColumn id="15" name="Q14"/>
+    <tableColumn id="16" name="Q15"/>
+    <tableColumn id="17" name="Q16"/>
+    <tableColumn id="18" name="Q17"/>
+    <tableColumn id="19" name="Q18"/>
+    <tableColumn id="20" name="Q19"/>
+    <tableColumn id="21" name="Q20"/>
+    <tableColumn id="22" name="Total"/>
+    <tableColumn id="23" name="% Correct"/>
+    <tableColumn id="24" name="z"/>
+    <tableColumn id="25" name="T"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -642,86 +700,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y54"/>
+  <dimension ref="A1:Y69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3035,257 +3093,804 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:21">
       <c r="A34" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>4</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U34" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21">
       <c r="A35" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B35">
-        <v>10.833</v>
+        <v>0.533</v>
       </c>
       <c r="C35">
-        <v>54.167</v>
+        <v>0.533</v>
       </c>
       <c r="D35">
-        <v>-0.01</v>
+        <v>0.433</v>
       </c>
       <c r="E35">
-        <v>49.9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>0.633</v>
+      </c>
+      <c r="F35">
+        <v>0.5</v>
+      </c>
+      <c r="G35">
+        <v>0.5669999999999999</v>
+      </c>
+      <c r="H35">
+        <v>0.433</v>
+      </c>
+      <c r="I35">
+        <v>0.4</v>
+      </c>
+      <c r="J35">
+        <v>0.5</v>
+      </c>
+      <c r="K35">
+        <v>0.633</v>
+      </c>
+      <c r="L35">
+        <v>0.5669999999999999</v>
+      </c>
+      <c r="M35">
+        <v>0.633</v>
+      </c>
+      <c r="N35">
+        <v>0.7</v>
+      </c>
+      <c r="O35">
+        <v>0.333</v>
+      </c>
+      <c r="P35">
+        <v>0.633</v>
+      </c>
+      <c r="Q35">
+        <v>0.2</v>
+      </c>
+      <c r="R35">
+        <v>0.733</v>
+      </c>
+      <c r="S35">
+        <v>0.5669999999999999</v>
+      </c>
+      <c r="T35">
+        <v>0.8</v>
+      </c>
+      <c r="U35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21">
       <c r="A36" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B36">
-        <v>7</v>
+        <v>0.8</v>
       </c>
       <c r="C36">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>0.8</v>
+      </c>
+      <c r="D36">
+        <v>0.9</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>0.7</v>
+      </c>
+      <c r="H36">
+        <v>0.5</v>
+      </c>
+      <c r="I36">
+        <v>0.7</v>
+      </c>
+      <c r="J36">
+        <v>0.9</v>
+      </c>
+      <c r="K36">
+        <v>0.5</v>
+      </c>
+      <c r="L36">
+        <v>0.8</v>
+      </c>
+      <c r="M36">
+        <v>0.7</v>
+      </c>
+      <c r="N36">
+        <v>0.9</v>
+      </c>
+      <c r="O36">
+        <v>0.7</v>
+      </c>
+      <c r="P36">
+        <v>0.8</v>
+      </c>
+      <c r="Q36">
+        <v>0.4</v>
+      </c>
+      <c r="R36">
+        <v>1</v>
+      </c>
+      <c r="S36">
+        <v>0.6</v>
+      </c>
+      <c r="T36">
+        <v>0.9</v>
+      </c>
+      <c r="U36">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21">
       <c r="A37" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B37">
+        <v>0.1</v>
+      </c>
+      <c r="C37">
+        <v>0.2</v>
+      </c>
+      <c r="D37">
+        <v>0.3</v>
+      </c>
+      <c r="E37">
+        <v>0.1</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0.6</v>
+      </c>
+      <c r="H37">
+        <v>0.1</v>
+      </c>
+      <c r="I37">
+        <v>0.3</v>
+      </c>
+      <c r="J37">
+        <v>0.1</v>
+      </c>
+      <c r="K37">
+        <v>0.9</v>
+      </c>
+      <c r="L37">
+        <v>0.4</v>
+      </c>
+      <c r="M37">
+        <v>0.5</v>
+      </c>
+      <c r="N37">
+        <v>0.4</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <v>0.3</v>
+      </c>
+      <c r="Q37">
+        <v>0.1</v>
+      </c>
+      <c r="R37">
+        <v>0.3</v>
+      </c>
+      <c r="S37">
+        <v>0.7</v>
+      </c>
+      <c r="T37">
+        <v>0.7</v>
+      </c>
+      <c r="U37">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21">
+      <c r="A39" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I39" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C37">
+      <c r="J39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U39" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21">
+      <c r="A40" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40">
+        <v>0.7000000000000001</v>
+      </c>
+      <c r="C40">
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="D40">
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="E40">
+        <v>0.9</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>0.09999999999999998</v>
+      </c>
+      <c r="H40">
+        <v>0.4</v>
+      </c>
+      <c r="I40">
+        <v>0.4</v>
+      </c>
+      <c r="J40">
+        <v>0.8</v>
+      </c>
+      <c r="K40">
+        <v>-0.4</v>
+      </c>
+      <c r="L40">
+        <v>0.4</v>
+      </c>
+      <c r="M40">
+        <v>0.2</v>
+      </c>
+      <c r="N40">
+        <v>0.5</v>
+      </c>
+      <c r="O40">
+        <v>0.7</v>
+      </c>
+      <c r="P40">
+        <v>0.5</v>
+      </c>
+      <c r="Q40">
+        <v>0.3</v>
+      </c>
+      <c r="R40">
+        <v>0.7</v>
+      </c>
+      <c r="S40">
+        <v>-0.09999999999999998</v>
+      </c>
+      <c r="T40">
+        <v>0.2000000000000001</v>
+      </c>
+      <c r="U40">
+        <v>-0.4999999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21">
+      <c r="A41" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41">
+        <v>0.61</v>
+      </c>
+      <c r="C41">
+        <v>0.498</v>
+      </c>
+      <c r="D41">
+        <v>0.529</v>
+      </c>
+      <c r="E41">
+        <v>0.699</v>
+      </c>
+      <c r="F41">
+        <v>0.717</v>
+      </c>
+      <c r="G41">
+        <v>0.185</v>
+      </c>
+      <c r="H41">
+        <v>0.398</v>
+      </c>
+      <c r="I41">
+        <v>0.399</v>
+      </c>
+      <c r="J41">
+        <v>0.624</v>
+      </c>
+      <c r="K41">
+        <v>-0.287</v>
+      </c>
+      <c r="L41">
+        <v>0.429</v>
+      </c>
+      <c r="M41">
+        <v>0.158</v>
+      </c>
+      <c r="N41">
+        <v>0.457</v>
+      </c>
+      <c r="O41">
+        <v>0.645</v>
+      </c>
+      <c r="P41">
+        <v>0.506</v>
+      </c>
+      <c r="Q41">
+        <v>0.396</v>
+      </c>
+      <c r="R41">
+        <v>0.6879999999999999</v>
+      </c>
+      <c r="S41">
+        <v>-0.06</v>
+      </c>
+      <c r="T41">
+        <v>0.256</v>
+      </c>
+      <c r="U41">
+        <v>-0.345</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21">
+      <c r="A43" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1</v>
+      </c>
+      <c r="D43" s="1">
+        <v>2</v>
+      </c>
+      <c r="E43" s="1">
+        <v>3</v>
+      </c>
+      <c r="F43" s="1">
+        <v>4</v>
+      </c>
+      <c r="G43" s="1">
+        <v>5</v>
+      </c>
+      <c r="H43" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21">
+      <c r="A44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21">
+      <c r="A45" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" t="s">
+        <v>18</v>
+      </c>
+      <c r="G45" t="s">
+        <v>19</v>
+      </c>
+      <c r="H45" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21">
+      <c r="A46" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" t="s">
+        <v>12</v>
+      </c>
+      <c r="E46" t="s">
+        <v>18</v>
+      </c>
+      <c r="F46" t="s">
+        <v>19</v>
+      </c>
+      <c r="G46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B50">
+        <v>10.833</v>
+      </c>
+      <c r="C50">
+        <v>54.167</v>
+      </c>
+      <c r="D50">
+        <v>-0.01</v>
+      </c>
+      <c r="E50">
+        <v>49.9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51">
+        <v>7</v>
+      </c>
+      <c r="C51">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52">
+        <v>8</v>
+      </c>
+      <c r="C52">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B38">
+    <row r="53" spans="1:5">
+      <c r="A53" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53">
         <v>11</v>
       </c>
-      <c r="C38">
+      <c r="C53">
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B39">
+    <row r="54" spans="1:5">
+      <c r="A54" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54">
         <v>13</v>
       </c>
-      <c r="C39">
+      <c r="C54">
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B40">
+    <row r="55" spans="1:5">
+      <c r="A55" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B55">
         <v>19</v>
       </c>
-      <c r="C40">
+      <c r="C55">
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B41">
+    <row r="56" spans="1:5">
+      <c r="A56" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B56">
         <v>3</v>
       </c>
-      <c r="C41">
+      <c r="C56">
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B42">
+    <row r="57" spans="1:5">
+      <c r="A57" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B57">
         <v>17</v>
       </c>
-      <c r="C42">
+      <c r="C57">
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B43">
+    <row r="58" spans="1:5">
+      <c r="A58" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B58">
         <v>3.578</v>
       </c>
-      <c r="C43">
+      <c r="C58">
         <v>17.892</v>
       </c>
-      <c r="D43">
+      <c r="D58">
         <v>0.998</v>
       </c>
-      <c r="E43">
+      <c r="E58">
         <v>9.984</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B44">
+    <row r="59" spans="1:5">
+      <c r="A59" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B59">
         <v>3.64</v>
       </c>
-      <c r="C44">
+      <c r="C59">
         <v>18.198</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B45">
+    <row r="60" spans="1:5">
+      <c r="A60" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B60">
         <v>12.806</v>
       </c>
-      <c r="C45">
+      <c r="C60">
         <v>3.201</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B46">
+    <row r="61" spans="1:5">
+      <c r="A61" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B61">
         <v>13.247</v>
       </c>
-      <c r="C46">
+      <c r="C61">
         <v>3.312</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B47">
+    <row r="62" spans="1:5">
+      <c r="A62" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B62">
         <v>2.5</v>
       </c>
-      <c r="C47">
+      <c r="C62">
         <v>12.5</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B48">
+    <row r="63" spans="1:5">
+      <c r="A63" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B63">
         <v>30</v>
       </c>
-      <c r="C48">
+      <c r="C63">
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B49">
+    <row r="64" spans="1:5">
+      <c r="A64" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B64">
         <v>0.07000000000000001</v>
       </c>
-      <c r="C49">
+      <c r="C64">
         <v>0.07000000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B50">
+    <row r="65" spans="1:3">
+      <c r="A65" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B65">
         <v>0.427</v>
       </c>
-      <c r="C50">
+      <c r="C65">
         <v>0.427</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B51">
+    <row r="66" spans="1:3">
+      <c r="A66" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B66">
         <v>0.164</v>
       </c>
-      <c r="C51">
+      <c r="C66">
         <v>0.164</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B52">
+    <row r="67" spans="1:3">
+      <c r="A67" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B67">
         <v>-0.193</v>
       </c>
-      <c r="C52">
+      <c r="C67">
         <v>-0.193</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B53">
+    <row r="68" spans="1:3">
+      <c r="A68" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B68">
         <v>0.833</v>
       </c>
-      <c r="C53">
+      <c r="C68">
         <v>0.833</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B54">
+    <row r="69" spans="1:3">
+      <c r="A69" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B69">
         <v>-0.232</v>
       </c>
-      <c r="C54">
+      <c r="C69">
         <v>-0.232</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>